<commit_message>
Chỉnh sửa mức điểm tối thiểu
Tính cả trường hợp làm tròn từ 0.05 lên 0.1
</commit_message>
<xml_diff>
--- a/2017-2/HOW TO GET 4.0 GPA.xlsx
+++ b/2017-2/HOW TO GET 4.0 GPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HOW TO GET 4.0 GPA\HOW-TO-GET-4.0-GPA\2017-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{19C87F61-DDF1-4469-9469-0868587BFFEE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F61444F7-3E30-4F8D-874F-C780D9558F64}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6765" xr2:uid="{AA75DEA7-1606-48DA-941E-33132A4E3DAD}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>HOW TO GET GPA 4.0</t>
   </si>
   <si>
-    <t>Mức điểm tối thiểu</t>
-  </si>
-  <si>
     <t>Timeline</t>
   </si>
   <si>
@@ -247,6 +244,9 @@
   </si>
   <si>
     <t>Ôn tập lý thuyết, viết tài liệu</t>
+  </si>
+  <si>
+    <t>Mức điểm tối thiểu (min = 3)</t>
   </si>
 </sst>
 </file>
@@ -505,6 +505,21 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -533,21 +548,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -702,7 +702,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -732,6 +731,7 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1116,26 +1116,26 @@
     <tableColumn id="4" xr3:uid="{8C1600C9-F108-46CE-B6E5-D6E622D71D13}" name="Kíp" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{8AC9E266-9D7C-428E-BFF4-0C46630AC6C1}" name="Ghi chú" dataDxfId="15"/>
     <tableColumn id="6" xr3:uid="{142F0582-89C2-4BAA-AC18-7A254F0B1622}" name="Giữa kỳ" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{DC2B866C-03EE-4027-8D7E-9744616EC2CC}" name="A/A+" dataDxfId="5">
-      <calculatedColumnFormula>CEILING((8.5 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{DC2B866C-03EE-4027-8D7E-9744616EC2CC}" name="A/A+" dataDxfId="6">
+      <calculatedColumnFormula>CEILING((8.5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{379E9C9F-943E-4CCC-A684-4A1BFA762DE3}" name="B+" dataDxfId="6">
-      <calculatedColumnFormula>CEILING((8 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{379E9C9F-943E-4CCC-A684-4A1BFA762DE3}" name="B+" dataDxfId="5">
+      <calculatedColumnFormula>CEILING((8 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{7EF678EE-3B63-4D90-9423-F3599A3CD227}" name="B" dataDxfId="4">
-      <calculatedColumnFormula>CEILING((7 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+      <calculatedColumnFormula>CEILING((7 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" xr3:uid="{6FE0E8B9-6D68-46FE-ACA5-4AB7AFE03433}" name="C+" dataDxfId="3">
-      <calculatedColumnFormula>CEILING((6.5 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+      <calculatedColumnFormula>CEILING((6.5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{118CBB8C-7160-4716-B6EF-85AD916D3E71}" name="C" dataDxfId="2">
-      <calculatedColumnFormula>CEILING((5.5 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+      <calculatedColumnFormula>CEILING((5.5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="12" xr3:uid="{18DDC3A9-418D-4319-B61E-455D319E22B2}" name="D+" dataDxfId="1">
-      <calculatedColumnFormula>CEILING((5 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+      <calculatedColumnFormula>CEILING((5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{00E7FF25-4B40-465E-8915-295D8A67CBDE}" name="D" dataDxfId="0">
-      <calculatedColumnFormula>CEILING((4 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
+      <calculatedColumnFormula>CEILING((4 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1454,7 +1454,7 @@
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:M1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1473,51 +1473,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="A2" s="18"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
       <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1564,10 +1564,10 @@
         <v>43242</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1588,41 +1588,41 @@
         <v>5</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G12" si="0">CEILING((8.5 - F4*0.3)/0.7, 0.5)</f>
+        <f>CEILING((8.5 - 0.05 - F4*0.3)/0.7, 0.5)</f>
         <v>10</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" ref="H4:H12" si="1">CEILING((8 - F4*0.3)/0.7, 0.5)</f>
+        <f t="shared" ref="H4:H12" si="0">CEILING((8 - 0.05 - F4*0.3)/0.7, 0.5)</f>
         <v>9.5</v>
       </c>
       <c r="I4" s="3">
-        <f t="shared" ref="I4:I12" si="2">CEILING((7 - F4*0.3)/0.7, 0.5)</f>
+        <f t="shared" ref="I4:I12" si="1">CEILING((7 - 0.05 - F4*0.3)/0.7, 0.5)</f>
         <v>8</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J12" si="3">CEILING((6.5 - F4*0.3)/0.7, 0.5)</f>
+        <f t="shared" ref="J4:J12" si="2">CEILING((6.5 - 0.05 - F4*0.3)/0.7, 0.5)</f>
         <v>7.5</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" ref="K4:K12" si="4">CEILING((5.5 - F4*0.3)/0.7, 0.5)</f>
+        <f t="shared" ref="K4:K12" si="3">CEILING((5.5 - 0.05 - F4*0.3)/0.7, 0.5)</f>
         <v>6</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L12" si="5">CEILING((5 - F4*0.3)/0.7, 0.5)</f>
+        <f t="shared" ref="L4:L12" si="4">CEILING((5 - 0.05 - F4*0.3)/0.7, 0.5)</f>
         <v>5</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M4:M12" si="6">CEILING((4 - F4*0.3)/0.7, 0.5)</f>
-        <v>4</v>
+        <f t="shared" ref="M4:M12" si="5">CEILING((4 - 0.05 - F4*0.3)/0.7, 0.5)</f>
+        <v>3.5</v>
       </c>
       <c r="N4" s="4">
         <v>43243</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1643,41 +1643,41 @@
         <v>9</v>
       </c>
       <c r="G5" s="5">
+        <f t="shared" ref="G4:G12" si="6">CEILING((8.5 - 0.05 - F5*0.3)/0.7, 0.5)</f>
+        <v>8.5</v>
+      </c>
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="H5" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="I5" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I5" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J5" s="3">
         <f t="shared" si="2"/>
-        <v>6.5</v>
-      </c>
-      <c r="J5" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="K5" s="3">
         <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-      <c r="K5" s="3">
+        <v>4</v>
+      </c>
+      <c r="L5" s="3">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L5" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="M5" s="3">
         <f t="shared" si="5"/>
-        <v>3.5</v>
-      </c>
-      <c r="M5" s="3">
-        <f>CEILING((4 - F5*0.3)/0.7, 0.5)</f>
         <v>2</v>
       </c>
       <c r="N5" s="4">
         <v>43244</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1698,41 +1698,41 @@
         <v>8</v>
       </c>
       <c r="G6" s="5">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H6" s="3">
+        <v>8</v>
+      </c>
+      <c r="I6" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I6" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J6" s="3">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="J6" s="3">
+        <v>6</v>
+      </c>
+      <c r="K6" s="3">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="K6" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="L6" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
-      </c>
-      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="M6" s="3">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="M6" s="3">
-        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="N6" s="4">
         <v>43245</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1753,41 +1753,41 @@
         <v>8</v>
       </c>
       <c r="G7" s="5">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H7" s="3">
+        <v>8</v>
+      </c>
+      <c r="I7" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I7" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J7" s="3">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="J7" s="3">
+        <v>6</v>
+      </c>
+      <c r="K7" s="3">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="K7" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="L7" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
-      </c>
-      <c r="L7" s="3">
+        <v>4</v>
+      </c>
+      <c r="M7" s="3">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="M7" s="3">
-        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="N7" s="4">
         <v>43246</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1808,41 +1808,41 @@
         <v>10</v>
       </c>
       <c r="G8" s="5">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H8" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="I8" s="3">
         <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="I8" s="3">
+        <v>6</v>
+      </c>
+      <c r="J8" s="3">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J8" s="3">
+        <v>5</v>
+      </c>
+      <c r="K8" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K8" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L8" s="3">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L8" s="3">
+        <v>3</v>
+      </c>
+      <c r="M8" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M8" s="3">
-        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="N8" s="4">
         <v>43247</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,41 +1863,41 @@
         <v>9</v>
       </c>
       <c r="G9" s="5">
+        <f t="shared" si="6"/>
+        <v>8.5</v>
+      </c>
+      <c r="H9" s="3">
         <f t="shared" si="0"/>
-        <v>8.5</v>
-      </c>
-      <c r="H9" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="I9" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I9" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J9" s="3">
         <f t="shared" si="2"/>
-        <v>6.5</v>
-      </c>
-      <c r="J9" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="K9" s="3">
         <f t="shared" si="3"/>
-        <v>5.5</v>
-      </c>
-      <c r="K9" s="3">
+        <v>4</v>
+      </c>
+      <c r="L9" s="3">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L9" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="M9" s="3">
         <f t="shared" si="5"/>
-        <v>3.5</v>
-      </c>
-      <c r="M9" s="3">
-        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="N9" s="4">
         <v>43248</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,41 +1918,41 @@
         <v>8</v>
       </c>
       <c r="G10" s="5">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="H10" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="H10" s="3">
+        <v>8</v>
+      </c>
+      <c r="I10" s="3">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="I10" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="J10" s="3">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="J10" s="3">
+        <v>6</v>
+      </c>
+      <c r="K10" s="3">
         <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="K10" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="L10" s="3">
         <f t="shared" si="4"/>
-        <v>4.5</v>
-      </c>
-      <c r="L10" s="3">
+        <v>4</v>
+      </c>
+      <c r="M10" s="3">
         <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="M10" s="3">
-        <f t="shared" si="6"/>
         <v>2.5</v>
       </c>
       <c r="N10" s="4">
         <v>43249</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,41 +1973,41 @@
         <v>10</v>
       </c>
       <c r="G11" s="5">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H11" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="I11" s="3">
         <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="I11" s="3">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J11" s="3">
+        <v>5</v>
+      </c>
+      <c r="K11" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K11" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L11" s="3">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L11" s="3">
+        <v>3</v>
+      </c>
+      <c r="M11" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M11" s="3">
-        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="N11" s="4">
         <v>43250</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2028,67 +2028,67 @@
         <v>10</v>
       </c>
       <c r="G12" s="5">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H12" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="I12" s="3">
         <f t="shared" si="1"/>
-        <v>7.5</v>
-      </c>
-      <c r="I12" s="3">
+        <v>6</v>
+      </c>
+      <c r="J12" s="3">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="J12" s="3">
+        <v>5</v>
+      </c>
+      <c r="K12" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
-      <c r="K12" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="L12" s="3">
+        <v>3</v>
+      </c>
+      <c r="M12" s="3">
         <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="M12" s="3">
-        <f t="shared" si="6"/>
         <v>1.5</v>
       </c>
       <c r="N12" s="4">
         <v>43251</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
+      <c r="A13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="4">
         <v>43252</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2098,29 +2098,29 @@
       <c r="B14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="22"/>
+      <c r="C14" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="27"/>
       <c r="M14" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N14" s="4">
         <v>43253</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2130,29 +2130,29 @@
       <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
+      <c r="C15" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
       <c r="M15" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N15" s="4">
         <v>43254</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P15" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2162,29 +2162,29 @@
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
+      <c r="C16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="21"/>
       <c r="M16" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N16" s="4">
         <v>43255</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2194,29 +2194,29 @@
       <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="19"/>
+      <c r="C17" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="24"/>
       <c r="M17" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N17" s="4">
         <v>43256</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2226,29 +2226,29 @@
       <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
+      <c r="C18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
       <c r="M18" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N18" s="4">
         <v>43257</v>
       </c>
       <c r="O18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P18" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2258,29 +2258,29 @@
       <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="19"/>
+      <c r="C19" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
       <c r="M19" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N19" s="4">
         <v>43258</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2290,29 +2290,29 @@
       <c r="B20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
+      <c r="C20" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="21"/>
       <c r="M20" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N20" s="4">
         <v>43259</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2322,101 +2322,101 @@
       <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
+      <c r="C21" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24"/>
       <c r="M21" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N21" s="4">
         <v>43260</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="16"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="21"/>
       <c r="M22" s="12"/>
       <c r="N22" s="4">
         <v>43261</v>
       </c>
       <c r="O22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="P22" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="P22" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="19"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="24"/>
       <c r="M23" s="10"/>
       <c r="N23" s="4">
         <v>43262</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="16"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="21"/>
       <c r="M24" s="12"/>
       <c r="N24" s="4">
         <v>43263</v>
       </c>
       <c r="O24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P24" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2432,11 +2432,6 @@
     <filterColumn colId="10" showButton="0"/>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="A2:F2"/>
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C18:L18"/>
     <mergeCell ref="C19:L19"/>
@@ -2448,6 +2443,11 @@
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C20:L20"/>
     <mergeCell ref="C21:L21"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="20" scale="38" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Chỉnh lại trang in
</commit_message>
<xml_diff>
--- a/2017-2/HOW TO GET 4.0 GPA.xlsx
+++ b/2017-2/HOW TO GET 4.0 GPA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HOW TO GET 4.0 GPA\HOW-TO-GET-4.0-GPA\2017-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F61444F7-3E30-4F8D-874F-C780D9558F64}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1C25334A-194D-48DB-9E11-3E835AB0C0D0}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="6765" xr2:uid="{AA75DEA7-1606-48DA-941E-33132A4E3DAD}"/>
   </bookViews>
@@ -505,6 +505,36 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -518,36 +548,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -557,208 +557,6 @@
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0"/>
-        </left>
-        <right style="thin">
-          <color theme="0"/>
-        </right>
-        <top style="thin">
-          <color theme="0"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -892,6 +690,208 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1116,25 +1116,25 @@
     <tableColumn id="4" xr3:uid="{8C1600C9-F108-46CE-B6E5-D6E622D71D13}" name="Kíp" dataDxfId="16"/>
     <tableColumn id="5" xr3:uid="{8AC9E266-9D7C-428E-BFF4-0C46630AC6C1}" name="Ghi chú" dataDxfId="15"/>
     <tableColumn id="6" xr3:uid="{142F0582-89C2-4BAA-AC18-7A254F0B1622}" name="Giữa kỳ" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{DC2B866C-03EE-4027-8D7E-9744616EC2CC}" name="A/A+" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{DC2B866C-03EE-4027-8D7E-9744616EC2CC}" name="A/A+" dataDxfId="13">
       <calculatedColumnFormula>CEILING((8.5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{379E9C9F-943E-4CCC-A684-4A1BFA762DE3}" name="B+" dataDxfId="5">
+    <tableColumn id="8" xr3:uid="{379E9C9F-943E-4CCC-A684-4A1BFA762DE3}" name="B+" dataDxfId="12">
       <calculatedColumnFormula>CEILING((8 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7EF678EE-3B63-4D90-9423-F3599A3CD227}" name="B" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{7EF678EE-3B63-4D90-9423-F3599A3CD227}" name="B" dataDxfId="11">
       <calculatedColumnFormula>CEILING((7 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{6FE0E8B9-6D68-46FE-ACA5-4AB7AFE03433}" name="C+" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{6FE0E8B9-6D68-46FE-ACA5-4AB7AFE03433}" name="C+" dataDxfId="10">
       <calculatedColumnFormula>CEILING((6.5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{118CBB8C-7160-4716-B6EF-85AD916D3E71}" name="C" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{118CBB8C-7160-4716-B6EF-85AD916D3E71}" name="C" dataDxfId="9">
       <calculatedColumnFormula>CEILING((5.5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{18DDC3A9-418D-4319-B61E-455D319E22B2}" name="D+" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{18DDC3A9-418D-4319-B61E-455D319E22B2}" name="D+" dataDxfId="8">
       <calculatedColumnFormula>CEILING((5 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00E7FF25-4B40-465E-8915-295D8A67CBDE}" name="D" dataDxfId="0">
+    <tableColumn id="13" xr3:uid="{00E7FF25-4B40-465E-8915-295D8A67CBDE}" name="D" dataDxfId="7">
       <calculatedColumnFormula>CEILING((4 - 0.05 - F4*0.3)/0.7, 0.5)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1143,12 +1143,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EE4C26E0-A223-43EE-97B8-2BEB3B6992C0}" name="Table5" displayName="Table5" ref="N2:P24" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" headerRowCellStyle="Note">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EE4C26E0-A223-43EE-97B8-2BEB3B6992C0}" name="Table5" displayName="Table5" ref="N2:P24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" tableBorderDxfId="3" headerRowCellStyle="Note">
   <autoFilter ref="N2:P24" xr:uid="{7CD1D58A-939F-4BC2-A3EC-DE16F4C53EE2}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C011BFCD-21A5-405C-BC11-51EBAC3C17F4}" name="Ngày" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{86235CD0-F848-4F39-BCB8-FB7F681E0569}" name="Công việc" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{3AB7C239-9F89-42B8-959F-CB84A1470F24}" name="Mô tả" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{C011BFCD-21A5-405C-BC11-51EBAC3C17F4}" name="Ngày" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{86235CD0-F848-4F39-BCB8-FB7F681E0569}" name="Công việc" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{3AB7C239-9F89-42B8-959F-CB84A1470F24}" name="Mô tả" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1451,65 +1451,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{709E60FE-6D3A-44D1-9CF1-2149ACE2EC29}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" style="1" customWidth="1"/>
-    <col min="7" max="13" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="13" width="4.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="66.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="32.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="37.140625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="14" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="17" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1643,7 +1644,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" ref="G4:G12" si="6">CEILING((8.5 - 0.05 - F5*0.3)/0.7, 0.5)</f>
+        <f t="shared" ref="G5:G12" si="6">CEILING((8.5 - 0.05 - F5*0.3)/0.7, 0.5)</f>
         <v>8.5</v>
       </c>
       <c r="H5" s="3">
@@ -2066,21 +2067,21 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
       <c r="N13" s="4">
         <v>43252</v>
       </c>
@@ -2098,18 +2099,18 @@
       <c r="B14" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="27"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
       <c r="M14" s="8" t="s">
         <v>43</v>
       </c>
@@ -2130,18 +2131,18 @@
       <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
       <c r="M15" s="13" t="s">
         <v>44</v>
       </c>
@@ -2162,18 +2163,18 @@
       <c r="B16" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="21"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="12" t="s">
         <v>44</v>
       </c>
@@ -2194,18 +2195,18 @@
       <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
       <c r="M17" s="10" t="s">
         <v>44</v>
       </c>
@@ -2226,18 +2227,18 @@
       <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="16"/>
       <c r="M18" s="12" t="s">
         <v>44</v>
       </c>
@@ -2258,18 +2259,18 @@
       <c r="B19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="19"/>
       <c r="M19" s="10" t="s">
         <v>44</v>
       </c>
@@ -2290,18 +2291,18 @@
       <c r="B20" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="21"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="12" t="s">
         <v>44</v>
       </c>
@@ -2322,18 +2323,18 @@
       <c r="B21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="19"/>
       <c r="M21" s="10" t="s">
         <v>44</v>
       </c>
@@ -2350,16 +2351,16 @@
     <row r="22" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="21"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="12"/>
       <c r="N22" s="4">
         <v>43261</v>
@@ -2374,16 +2375,16 @@
     <row r="23" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="24"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="19"/>
       <c r="M23" s="10"/>
       <c r="N23" s="4">
         <v>43262</v>
@@ -2398,16 +2399,16 @@
     <row r="24" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="21"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="16"/>
       <c r="M24" s="12"/>
       <c r="N24" s="4">
         <v>43263</v>
@@ -2432,6 +2433,11 @@
     <filterColumn colId="10" showButton="0"/>
   </autoFilter>
   <mergeCells count="16">
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="A13:M13"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="A2:F2"/>
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C18:L18"/>
     <mergeCell ref="C19:L19"/>
@@ -2443,14 +2449,9 @@
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C20:L20"/>
     <mergeCell ref="C21:L21"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="A13:M13"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="A2:F2"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="20" scale="38" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="1.8" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="81" orientation="landscape" r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>

</xml_diff>